<commit_message>
finished PBMC20k guided analysis up to SJARACNe network construction section
</commit_message>
<xml_diff>
--- a/docs/tests/Ref/PBMC_markers.xlsx
+++ b/docs/tests/Ref/PBMC_markers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lding/Git/scMINER/docs/tests/Ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D58A600-1077-7F4E-B22D-C6DABCF494E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C15B40-9481-B843-8F86-8B119CBAB459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58860" yWindow="500" windowWidth="28660" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52140" yWindow="-3680" windowWidth="28660" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Markers_10_cell_types_PBMC_12k" sheetId="9" r:id="rId1"/>
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7B1221-3BCF-6344-A007-709E81DDCC11}">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A75" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C91" sqref="A1:C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3239,8 +3239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DC9C9C-A5E7-584A-B184-259BDB222503}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>